<commit_message>
Versão api com testes
</commit_message>
<xml_diff>
--- a/doc/FeiraLivre.xlsx
+++ b/doc/FeiraLivre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilso\source\repos\Testes\desafio-feira\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A056CD07-6B10-4DDC-BA1E-35C270CA51B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F36A9D05-9633-4A3D-8739-62BE5A80E090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29175" yWindow="870" windowWidth="26910" windowHeight="14025" activeTab="1" xr2:uid="{60423FA2-57B6-4DF0-A819-FE6B2BE0B058}"/>
+    <workbookView xWindow="29175" yWindow="870" windowWidth="26910" windowHeight="14025" xr2:uid="{60423FA2-57B6-4DF0-A819-FE6B2BE0B058}"/>
   </bookViews>
   <sheets>
     <sheet name="DEINFO_AB_FEIRASLIVRES_2014_Var" sheetId="2" r:id="rId1"/>
@@ -11832,7 +11832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80A7A8A-5A53-4143-AC6C-FE96A57B87FF}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -12273,7 +12273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B71CF666-74A3-483A-B5A1-04E52C5C9492}">
   <dimension ref="A1:Q881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A863" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E878" sqref="E878"/>
     </sheetView>
   </sheetViews>

</xml_diff>